<commit_message>
intermediate commit; ModelWrapper now uses pandas
</commit_message>
<xml_diff>
--- a/tests/test_data/spreadsheets/bad-fixed.xlsx
+++ b/tests/test_data/spreadsheets/bad-fixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/work/programming/git-clones/dataprob/tests/test_data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DB5559D-9AC0-364F-807C-5DA2E1742343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE76BE82-C09C-9A43-A4B6-14EA02038ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2700" yWindow="2820" windowWidth="26440" windowHeight="15440" xr2:uid="{AE00FBF8-3830-3845-857E-C46D5BABC3ED}"/>
   </bookViews>
@@ -41,10 +41,10 @@
     <t>fixed</t>
   </si>
   <si>
-    <t>param</t>
+    <t>K1</t>
   </si>
   <si>
-    <t>K1</t>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -437,7 +437,7 @@
         <v>1.5</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>